<commit_message>
menambahkan list dan create barang
</commit_message>
<xml_diff>
--- a/##/data.xlsx
+++ b/##/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\e-man\##\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0313D73C-8103-4B51-A945-FF79E935A1C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F07832-B3C4-4563-B0D9-278DA2384D63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{E81758E1-20C1-4FCD-8767-51C80920AF6B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="2" xr2:uid="{E81758E1-20C1-4FCD-8767-51C80920AF6B}"/>
   </bookViews>
   <sheets>
     <sheet name="PEGAWAI" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="159">
   <si>
     <t>NO</t>
   </si>
@@ -343,12 +343,6 @@
     <t>001-BOS</t>
   </si>
   <si>
-    <t>11-06-2021</t>
-  </si>
-  <si>
-    <t>26-11-2021</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
@@ -476,6 +470,42 @@
   </si>
   <si>
     <t>iva-dwi-meilydiawati-spd-gr</t>
+  </si>
+  <si>
+    <t>PRS-BOS-2021</t>
+  </si>
+  <si>
+    <t>KAD-BOS-2021</t>
+  </si>
+  <si>
+    <t>SRA-BOS-2021</t>
+  </si>
+  <si>
+    <t>CPUKI-BOS-2021</t>
+  </si>
+  <si>
+    <t>CPURE-BOS-2021</t>
+  </si>
+  <si>
+    <t>MNR-BOS-2021</t>
+  </si>
+  <si>
+    <t>LTP-BOS-2021</t>
+  </si>
+  <si>
+    <t>MUI-BOS-2021</t>
+  </si>
+  <si>
+    <t>MUG-BOS-2021</t>
+  </si>
+  <si>
+    <t>KGG-BOS-2021</t>
+  </si>
+  <si>
+    <t>2021-6-11</t>
+  </si>
+  <si>
+    <t>2021-11-26</t>
   </si>
 </sst>
 </file>
@@ -839,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4A8F0A-B9F9-425D-B073-52501615F5A5}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -887,7 +917,7 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -907,7 +937,7 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -927,7 +957,7 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -947,7 +977,7 @@
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -967,7 +997,7 @@
         <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,7 +1017,7 @@
         <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,7 +1037,7 @@
         <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1027,7 +1057,7 @@
         <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1047,7 +1077,7 @@
         <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1067,7 +1097,7 @@
         <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1283,482 +1313,659 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47225827-A394-4E28-AD40-0F65E3C8E95A}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>70</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>72</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>73</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>74</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>75</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>76</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>77</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" t="s">
         <v>79</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>90</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>91</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>96</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>103</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" t="s">
         <v>104</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>106</v>
       </c>
-      <c r="K2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L2">
+      <c r="M2">
         <v>7300000</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>11</v>
+      </c>
+      <c r="P2">
+        <v>6</v>
+      </c>
+      <c r="Q2">
+        <v>2021</v>
+      </c>
+      <c r="S2" t="str">
+        <f>Q2&amp;"-"&amp;P2&amp;"-"&amp;O2</f>
+        <v>2021-6-11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" t="s">
         <v>80</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>90</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>92</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>97</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>103</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K3" t="s">
         <v>104</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>106</v>
       </c>
-      <c r="K3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L3">
+      <c r="M3">
         <v>1700000</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>11</v>
+      </c>
+      <c r="P3">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <v>2021</v>
+      </c>
+      <c r="S3" t="str">
+        <f t="shared" ref="S3:S12" si="0">Q3&amp;"-"&amp;P3&amp;"-"&amp;O3</f>
+        <v>2021-6-11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" t="s">
         <v>81</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>90</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>93</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>98</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>103</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>157</v>
+      </c>
+      <c r="K4" t="s">
         <v>104</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>106</v>
       </c>
-      <c r="K4" t="s">
-        <v>108</v>
-      </c>
-      <c r="L4">
+      <c r="M4">
         <v>4235000</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>11</v>
+      </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <v>2021</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="0"/>
+        <v>2021-6-11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" t="s">
         <v>82</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>90</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>94</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>99</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>103</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K5" t="s">
         <v>104</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>106</v>
       </c>
-      <c r="K5" t="s">
-        <v>108</v>
-      </c>
-      <c r="L5">
+      <c r="M5">
         <v>15000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>11</v>
+      </c>
+      <c r="P5">
+        <v>6</v>
+      </c>
+      <c r="Q5">
+        <v>2021</v>
+      </c>
+      <c r="S5" t="str">
+        <f t="shared" si="0"/>
+        <v>2021-6-11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" t="s">
         <v>83</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>90</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>92</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>100</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>103</v>
       </c>
-      <c r="I6" t="s">
-        <v>105</v>
-      </c>
       <c r="J6" t="s">
+        <v>158</v>
+      </c>
+      <c r="K6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L6" t="s">
         <v>106</v>
       </c>
-      <c r="K6" t="s">
-        <v>108</v>
-      </c>
-      <c r="L6">
+      <c r="M6">
         <v>1700000</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>26</v>
+      </c>
+      <c r="P6">
+        <v>11</v>
+      </c>
+      <c r="Q6">
+        <v>2021</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="0"/>
+        <v>2021-11-26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" t="s">
         <v>84</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>90</v>
-      </c>
-      <c r="F7" t="s">
-        <v>94</v>
       </c>
       <c r="G7" t="s">
         <v>94</v>
       </c>
       <c r="H7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" t="s">
         <v>103</v>
       </c>
-      <c r="I7" t="s">
-        <v>105</v>
-      </c>
       <c r="J7" t="s">
+        <v>158</v>
+      </c>
+      <c r="K7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L7" t="s">
         <v>106</v>
       </c>
-      <c r="K7" t="s">
-        <v>108</v>
-      </c>
-      <c r="L7">
+      <c r="M7">
         <v>3750000</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>26</v>
+      </c>
+      <c r="P7">
+        <v>11</v>
+      </c>
+      <c r="Q7">
+        <v>2021</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" si="0"/>
+        <v>2021-11-26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" t="s">
         <v>85</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>90</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>94</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>101</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>103</v>
       </c>
-      <c r="I8" t="s">
-        <v>105</v>
-      </c>
       <c r="J8" t="s">
+        <v>158</v>
+      </c>
+      <c r="K8" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" t="s">
         <v>106</v>
       </c>
-      <c r="K8" t="s">
-        <v>108</v>
-      </c>
-      <c r="L8">
+      <c r="M8">
         <v>6375000</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>26</v>
+      </c>
+      <c r="P8">
+        <v>11</v>
+      </c>
+      <c r="Q8">
+        <v>2021</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="0"/>
+        <v>2021-11-26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" t="s">
         <v>86</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>90</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>95</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>102</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>103</v>
       </c>
-      <c r="I9" t="s">
-        <v>105</v>
-      </c>
       <c r="J9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K9" t="s">
+        <v>104</v>
+      </c>
+      <c r="L9" t="s">
         <v>106</v>
       </c>
-      <c r="K9" t="s">
-        <v>108</v>
-      </c>
-      <c r="L9">
+      <c r="M9">
         <v>9850000</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>26</v>
+      </c>
+      <c r="P9">
+        <v>11</v>
+      </c>
+      <c r="Q9">
+        <v>2021</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="0"/>
+        <v>2021-11-26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" t="s">
         <v>87</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>75</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>90</v>
-      </c>
-      <c r="F10" t="s">
-        <v>94</v>
       </c>
       <c r="G10" t="s">
         <v>94</v>
       </c>
       <c r="H10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" t="s">
         <v>103</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
+        <v>158</v>
+      </c>
+      <c r="K10" t="s">
         <v>105</v>
       </c>
-      <c r="J10" t="s">
-        <v>107</v>
-      </c>
-      <c r="K10" t="s">
-        <v>108</v>
-      </c>
-      <c r="L10">
+      <c r="L10" t="s">
+        <v>106</v>
+      </c>
+      <c r="M10">
         <v>66000000</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>26</v>
+      </c>
+      <c r="P10">
+        <v>11</v>
+      </c>
+      <c r="Q10">
+        <v>2021</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="0"/>
+        <v>2021-11-26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" t="s">
         <v>88</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>90</v>
-      </c>
-      <c r="F11" t="s">
-        <v>94</v>
       </c>
       <c r="G11" t="s">
         <v>94</v>
       </c>
       <c r="H11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" t="s">
         <v>103</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
+        <v>158</v>
+      </c>
+      <c r="K11" t="s">
         <v>105</v>
       </c>
-      <c r="J11" t="s">
-        <v>107</v>
-      </c>
-      <c r="K11" t="s">
-        <v>108</v>
-      </c>
-      <c r="L11">
+      <c r="L11" t="s">
+        <v>106</v>
+      </c>
+      <c r="M11">
         <v>1650000</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>26</v>
+      </c>
+      <c r="P11">
+        <v>11</v>
+      </c>
+      <c r="Q11">
+        <v>2021</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="0"/>
+        <v>2021-11-26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" t="s">
         <v>89</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>90</v>
-      </c>
-      <c r="F12" t="s">
-        <v>94</v>
       </c>
       <c r="G12" t="s">
         <v>94</v>
       </c>
       <c r="H12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" t="s">
         <v>103</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
+        <v>158</v>
+      </c>
+      <c r="K12" t="s">
         <v>105</v>
       </c>
-      <c r="J12" t="s">
-        <v>107</v>
-      </c>
-      <c r="K12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L12">
+      <c r="L12" t="s">
+        <v>106</v>
+      </c>
+      <c r="M12">
         <v>2925000</v>
+      </c>
+      <c r="O12">
+        <v>26</v>
+      </c>
+      <c r="P12">
+        <v>11</v>
+      </c>
+      <c r="Q12">
+        <v>2021</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="0"/>
+        <v>2021-11-26</v>
       </c>
     </row>
   </sheetData>
@@ -1790,19 +1997,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>34</v>
@@ -1810,13 +2017,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E2" s="2">
         <v>44256</v>
@@ -1830,13 +2037,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E3" s="2">
         <v>44289</v>
@@ -1850,13 +2057,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E4" s="2">
         <v>44261</v>
@@ -1870,13 +2077,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E5" s="2">
         <v>1140081</v>
@@ -1890,13 +2097,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E6" s="2">
         <v>44386</v>
@@ -1936,27 +2143,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
         <v>130</v>
-      </c>
-      <c r="C2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" t="s">
-        <v>132</v>
       </c>
       <c r="E2">
         <v>150000</v>
@@ -1964,13 +2171,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E3">
         <v>150000</v>
@@ -1978,13 +2185,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E4">
         <v>150000</v>
@@ -1992,13 +2199,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E5">
         <v>150000</v>
@@ -2006,13 +2213,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E6">
         <v>150000</v>

</xml_diff>